<commit_message>
Add PDF versions of tables
</commit_message>
<xml_diff>
--- a/Data/Tables/Answer_Categorization.xlsx
+++ b/Data/Tables/Answer_Categorization.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058B7707-0EB3-4217-AF7A-AC35D24E398D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC565228-52CA-4B9D-ABB4-59564AF72A76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{01148236-0E3A-41EC-A501-E5FB4C731FFA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{01148236-0E3A-41EC-A501-E5FB4C731FFA}"/>
   </bookViews>
   <sheets>
     <sheet name="Gemini" sheetId="8" r:id="rId1"/>
@@ -732,10 +732,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{445C94FD-A203-4EF7-AC65-DA43755DEC7F}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:R50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="64" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C58" sqref="A46:C58"/>
+    <sheetView zoomScale="64" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R44" sqref="A1:R44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2037,16 +2040,20 @@
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:B11"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="52" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1082A0FD-D701-45E3-A926-C99FF4668F18}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:R45"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="65" workbookViewId="0">
-      <selection activeCell="D56" sqref="A47:D56"/>
+    <sheetView zoomScale="65" workbookViewId="0">
+      <selection activeCell="R44" sqref="A1:R44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3333,38 +3340,42 @@
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:B11"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="52" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69287C9A-8FAF-4C60-8531-B18B089A539E}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:R44"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="56" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" topLeftCell="B5" zoomScale="71" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.77734375" customWidth="1"/>
+    <col min="2" max="2" width="16.77734375" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" customWidth="1"/>
+    <col min="4" max="4" width="20.77734375" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" customWidth="1"/>
     <col min="6" max="6" width="23.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
     <col min="8" max="8" width="21.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.77734375" customWidth="1"/>
+    <col min="10" max="10" width="21.33203125" customWidth="1"/>
+    <col min="11" max="11" width="15.5546875" customWidth="1"/>
+    <col min="12" max="12" width="19.109375" customWidth="1"/>
+    <col min="13" max="13" width="20.33203125" customWidth="1"/>
+    <col min="14" max="14" width="14.5546875" customWidth="1"/>
     <col min="15" max="15" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18" customWidth="1"/>
     <col min="17" max="17" width="21.77734375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -4622,7 +4633,7 @@
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:B11"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="39" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>